<commit_message>
Added average calculation for benchmark 1
</commit_message>
<xml_diff>
--- a/benchmarks/lester_allocators/lester_results.xlsx
+++ b/benchmarks/lester_allocators/lester_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12105" tabRatio="594" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12105" tabRatio="594"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4811" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4923" uniqueCount="642">
   <si>
     <t>DS1: vector&lt;int&gt;</t>
   </si>
@@ -1953,6 +1953,9 @@
   </si>
   <si>
     <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>(Ratio new scheme to old scheme)</t>
   </si>
 </sst>
 </file>
@@ -2273,10 +2276,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH36" sqref="AH36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,15 +2301,18 @@
     <col min="15" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>46</v>
       </c>
       <c r="K1" t="s">
         <v>54</v>
       </c>
+      <c r="T1" t="s">
+        <v>641</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2352,8 +2358,29 @@
       <c r="R2" t="s">
         <v>16</v>
       </c>
+      <c r="U2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>17</v>
       </c>
@@ -2396,8 +2423,29 @@
       <c r="R3" t="s">
         <v>17</v>
       </c>
+      <c r="U3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>18</v>
       </c>
@@ -2416,8 +2464,17 @@
       <c r="R4" t="s">
         <v>18</v>
       </c>
+      <c r="W4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -2466,8 +2523,35 @@
       <c r="R5" t="s">
         <v>12</v>
       </c>
+      <c r="T5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>640</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -2516,8 +2600,43 @@
       <c r="R6">
         <v>0.82</v>
       </c>
+      <c r="T6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6">
+        <f>C6/L6</f>
+        <v>4.291666666666667</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:V16" si="0">D6/M6</f>
+        <v>4.5609756097560981</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ref="W6:W16" si="1">E6/N6</f>
+        <v>1.4390243902439024</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ref="X6:X16" si="2">F6/O6</f>
+        <v>5.021505376344086</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ref="Y6:Y16" si="3">G6/P6</f>
+        <v>3.531531531531531</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z16" si="4">H6/Q6</f>
+        <v>5.6233766233766236</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" ref="AA6:AA16" si="5">I6/R6</f>
+        <v>4.51219512195122</v>
+      </c>
+      <c r="AC6">
+        <f>AVERAGE(U6:AA16)</f>
+        <v>1.5867389231677316</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -2566,8 +2685,39 @@
       <c r="R7">
         <v>0.57999999999999996</v>
       </c>
+      <c r="T7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7:U16" si="6">C7/L7</f>
+        <v>2.8536585365853657</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="1"/>
+        <v>1.1052631578947367</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>3.7692307692307692</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="3"/>
+        <v>2.9285714285714284</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="4"/>
+        <v>3.9824561403508776</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="5"/>
+        <v>3.3793103448275863</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -2616,8 +2766,39 @@
       <c r="R8">
         <v>0.46</v>
       </c>
+      <c r="T8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>1.9444444444444444</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="1"/>
+        <v>1.1944444444444444</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="2"/>
+        <v>3.510204081632653</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="3"/>
+        <v>2.88</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="4"/>
+        <v>2.7954545454545454</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="5"/>
+        <v>2.3695652173913042</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -2666,8 +2847,39 @@
       <c r="R9">
         <v>0.4</v>
       </c>
+      <c r="T9" t="s">
+        <v>22</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="6"/>
+        <v>1.5555555555555558</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>1.342857142857143</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="1"/>
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>2.2926829268292681</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="3"/>
+        <v>2.15</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="4"/>
+        <v>1.9487179487179487</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="5"/>
+        <v>1.675</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -2716,8 +2928,39 @@
       <c r="R10">
         <v>0.37</v>
       </c>
+      <c r="T10" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="6"/>
+        <v>1.0857142857142859</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>1.0588235294117645</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="2"/>
+        <v>1.5526315789473684</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="3"/>
+        <v>1.4857142857142858</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="4"/>
+        <v>1.3783783783783785</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="5"/>
+        <v>1.2702702702702702</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -2766,8 +3009,39 @@
       <c r="R11">
         <v>0.35</v>
       </c>
+      <c r="T11" t="s">
+        <v>24</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="6"/>
+        <v>0.91428571428571437</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="1"/>
+        <v>0.79411764705882348</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="2"/>
+        <v>1.0833333333333335</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="3"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="4"/>
+        <v>1.0857142857142859</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="5"/>
+        <v>1.0285714285714287</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -2816,8 +3090,39 @@
       <c r="R12">
         <v>0.34</v>
       </c>
+      <c r="T12" t="s">
+        <v>25</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="6"/>
+        <v>0.85294117647058809</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="0"/>
+        <v>0.82352941176470595</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="1"/>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="2"/>
+        <v>0.94285714285714295</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="4"/>
+        <v>0.91176470588235292</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="5"/>
+        <v>0.91176470588235292</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -2866,8 +3171,39 @@
       <c r="R13">
         <v>0.34</v>
       </c>
+      <c r="T13" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="6"/>
+        <v>0.77142857142857157</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="0"/>
+        <v>0.79411764705882348</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="1"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="2"/>
+        <v>0.82857142857142851</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="3"/>
+        <v>0.93548387096774188</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="4"/>
+        <v>0.82857142857142851</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="5"/>
+        <v>0.85294117647058809</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -2916,8 +3252,39 @@
       <c r="R14">
         <v>0.34</v>
       </c>
+      <c r="T14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="6"/>
+        <v>0.79411764705882348</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="0"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="1"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="2"/>
+        <v>0.82352941176470595</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="3"/>
+        <v>0.90322580645161299</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="4"/>
+        <v>0.79411764705882348</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="5"/>
+        <v>0.85294117647058809</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
@@ -2966,8 +3333,39 @@
       <c r="R15">
         <v>0.35</v>
       </c>
+      <c r="T15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="6"/>
+        <v>0.79411764705882348</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="0"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="1"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="2"/>
+        <v>0.79411764705882348</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="3"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="4"/>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="5"/>
+        <v>0.74285714285714288</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>29</v>
       </c>
@@ -3016,13 +3414,44 @@
       <c r="R16">
         <v>0.34</v>
       </c>
+      <c r="T16" t="s">
+        <v>29</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="6"/>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="1"/>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="2"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="3"/>
+        <v>0.87096774193548399</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="4"/>
+        <v>0.72222222222222232</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="5"/>
+        <v>0.76470588235294112</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -3065,8 +3494,29 @@
       <c r="R19" t="s">
         <v>16</v>
       </c>
+      <c r="U19" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" t="s">
+        <v>14</v>
+      </c>
+      <c r="W19" t="s">
+        <v>14</v>
+      </c>
+      <c r="X19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>17</v>
       </c>
@@ -3109,8 +3559,29 @@
       <c r="R20" t="s">
         <v>17</v>
       </c>
+      <c r="U20" t="s">
+        <v>17</v>
+      </c>
+      <c r="V20" t="s">
+        <v>17</v>
+      </c>
+      <c r="W20" t="s">
+        <v>17</v>
+      </c>
+      <c r="X20" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>18</v>
       </c>
@@ -3129,8 +3600,17 @@
       <c r="R21" t="s">
         <v>18</v>
       </c>
+      <c r="W21" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -3179,8 +3659,35 @@
       <c r="R22" t="s">
         <v>12</v>
       </c>
+      <c r="T22" t="s">
+        <v>1</v>
+      </c>
+      <c r="U22" t="s">
+        <v>3</v>
+      </c>
+      <c r="V22" t="s">
+        <v>5</v>
+      </c>
+      <c r="W22" t="s">
+        <v>6</v>
+      </c>
+      <c r="X22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>640</v>
+      </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>19</v>
       </c>
@@ -3229,8 +3736,43 @@
       <c r="R23">
         <v>7.85</v>
       </c>
+      <c r="T23" t="s">
+        <v>19</v>
+      </c>
+      <c r="U23">
+        <f t="shared" ref="U23:U33" si="7">C23/L23</f>
+        <v>6.7734806629834248</v>
+      </c>
+      <c r="V23">
+        <f t="shared" ref="V23:V33" si="8">D23/M23</f>
+        <v>2.4065155807365439</v>
+      </c>
+      <c r="W23">
+        <f t="shared" ref="W23:W33" si="9">E23/N23</f>
+        <v>3.5785953177257519</v>
+      </c>
+      <c r="X23">
+        <f t="shared" ref="X23:X33" si="10">F23/O23</f>
+        <v>11.913957934990439</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" ref="Y23:Y33" si="11">G23/P23</f>
+        <v>10.653846153846153</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" ref="Z23:Z33" si="12">H23/Q23</f>
+        <v>10.331497797356828</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" ref="AA23:AA33" si="13">I23/R23</f>
+        <v>8.9210191082802552</v>
+      </c>
+      <c r="AC23">
+        <f>AVERAGE(U23:AA33)</f>
+        <v>5.9570466099328714</v>
+      </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -3279,8 +3821,39 @@
       <c r="R24">
         <v>8.58</v>
       </c>
+      <c r="T24" t="s">
+        <v>20</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="7"/>
+        <v>6.7574827321565616</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="8"/>
+        <v>2.5849056603773586</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="9"/>
+        <v>3.7281249999999999</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="10"/>
+        <v>3.8906657963446474</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="11"/>
+        <v>3.3934664246823956</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="12"/>
+        <v>9.2517552657973905</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="13"/>
+        <v>7.9487179487179489</v>
+      </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -3329,8 +3902,39 @@
       <c r="R25">
         <v>10.96</v>
       </c>
+      <c r="T25" t="s">
+        <v>21</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="7"/>
+        <v>3.0532663316582913</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="8"/>
+        <v>2.8017638036809815</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="9"/>
+        <v>3.3218785796105381</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="10"/>
+        <v>2.5799823243482103</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="11"/>
+        <v>2.132166705042597</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="12"/>
+        <v>7.752411575562701</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="13"/>
+        <v>6.5337591240875907</v>
+      </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -3379,8 +3983,39 @@
       <c r="R26">
         <v>11.27</v>
       </c>
+      <c r="T26" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="7"/>
+        <v>2.1975648977716515</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="8"/>
+        <v>3.1262485017978423</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="9"/>
+        <v>3.1096446700507614</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="10"/>
+        <v>2.0315972222222221</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="11"/>
+        <v>2.4394022234372152</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="12"/>
+        <v>7.7616191904047982</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="13"/>
+        <v>6.7657497781721387</v>
+      </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -3429,8 +4064,39 @@
       <c r="R27">
         <v>12.59</v>
       </c>
+      <c r="T27" t="s">
+        <v>23</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="7"/>
+        <v>1.9447828650029475</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="8"/>
+        <v>3.3878281622911692</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="9"/>
+        <v>3.4959919839679356</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="10"/>
+        <v>1.9799713876967098</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" si="11"/>
+        <v>2.0804727979274613</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="12"/>
+        <v>7.9627329192546581</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="13"/>
+        <v>6.7704527402700556</v>
+      </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -3479,8 +4145,39 @@
       <c r="R28">
         <v>13.49</v>
       </c>
+      <c r="T28" t="s">
+        <v>24</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="7"/>
+        <v>5.4472081218274111</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="8"/>
+        <v>3.986146095717884</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="9"/>
+        <v>3.4236047575480333</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="10"/>
+        <v>3.6730958749824016</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="11"/>
+        <v>3.5002251238181001</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="12"/>
+        <v>7.7487745098039209</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="13"/>
+        <v>7.2564862861378803</v>
+      </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>25</v>
       </c>
@@ -3529,8 +4226,39 @@
       <c r="R29">
         <v>13.14</v>
       </c>
+      <c r="T29" t="s">
+        <v>25</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="7"/>
+        <v>1.7348394768133175</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="8"/>
+        <v>4.7982385908726979</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="9"/>
+        <v>3.0608974358974361</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="10"/>
+        <v>3.947166921898928</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="11"/>
+        <v>4.5400252348240571</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="12"/>
+        <v>10.357320099255583</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="13"/>
+        <v>9.961948249619482</v>
+      </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -3579,8 +4307,39 @@
       <c r="R30">
         <v>14.06</v>
       </c>
+      <c r="T30" t="s">
+        <v>26</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="7"/>
+        <v>2.0761918689675345</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="8"/>
+        <v>9.6885311871227362</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="9"/>
+        <v>4.011504424778761</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="10"/>
+        <v>4.7202680067001674</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="11"/>
+        <v>4.6682712728302427</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="12"/>
+        <v>11.411730545876887</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="13"/>
+        <v>14.132290184921763</v>
+      </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>27</v>
       </c>
@@ -3629,8 +4388,39 @@
       <c r="R31">
         <v>21.63</v>
       </c>
+      <c r="T31" t="s">
+        <v>27</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="7"/>
+        <v>2.7169230769230768</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="8"/>
+        <v>8.2862218712988547</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="9"/>
+        <v>6.419926199261992</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="10"/>
+        <v>4.1674925668979181</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="11"/>
+        <v>4.4008643976229065</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="12"/>
+        <v>23.60159574468085</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="13"/>
+        <v>16.435968562182154</v>
+      </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -3679,8 +4469,39 @@
       <c r="R32">
         <v>36.090000000000003</v>
       </c>
+      <c r="T32" t="s">
+        <v>28</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="7"/>
+        <v>3.4984149708559156</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="8"/>
+        <v>9.3045060173523648</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="9"/>
+        <v>5.9914209115281505</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="10"/>
+        <v>3.7926050420168065</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="11"/>
+        <v>4.3585701191567372</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="12"/>
+        <v>11.360350492880615</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="13"/>
+        <v>13.308395677472983</v>
+      </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>29</v>
       </c>
@@ -3729,13 +4550,44 @@
       <c r="R33">
         <v>49.47</v>
       </c>
+      <c r="T33" t="s">
+        <v>29</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="7"/>
+        <v>3.3211081794195252</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="8"/>
+        <v>7.3419027632039171</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="9"/>
+        <v>3.7479909996785596</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="10"/>
+        <v>3.9659626320064989</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="11"/>
+        <v>5.4097522164128211</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="12"/>
+        <v>7.2354305991538146</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="13"/>
+        <v>10.519102486355367</v>
+      </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>13</v>
       </c>
@@ -3778,8 +4630,29 @@
       <c r="R36" t="s">
         <v>16</v>
       </c>
+      <c r="U36" t="s">
+        <v>13</v>
+      </c>
+      <c r="V36" t="s">
+        <v>14</v>
+      </c>
+      <c r="W36" t="s">
+        <v>14</v>
+      </c>
+      <c r="X36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>17</v>
       </c>
@@ -3822,8 +4695,29 @@
       <c r="R37" t="s">
         <v>17</v>
       </c>
+      <c r="U37" t="s">
+        <v>17</v>
+      </c>
+      <c r="V37" t="s">
+        <v>17</v>
+      </c>
+      <c r="W37" t="s">
+        <v>17</v>
+      </c>
+      <c r="X37" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>18</v>
       </c>
@@ -3842,8 +4736,17 @@
       <c r="R38" t="s">
         <v>18</v>
       </c>
+      <c r="W38" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>1</v>
       </c>
@@ -3892,8 +4795,35 @@
       <c r="R39" t="s">
         <v>12</v>
       </c>
+      <c r="T39" t="s">
+        <v>1</v>
+      </c>
+      <c r="U39" t="s">
+        <v>3</v>
+      </c>
+      <c r="V39" t="s">
+        <v>5</v>
+      </c>
+      <c r="W39" t="s">
+        <v>6</v>
+      </c>
+      <c r="X39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>640</v>
+      </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>19</v>
       </c>
@@ -3942,8 +4872,43 @@
       <c r="R40">
         <v>0.31</v>
       </c>
+      <c r="T40" t="s">
+        <v>19</v>
+      </c>
+      <c r="U40">
+        <f t="shared" ref="U40:U50" si="14">C40/L40</f>
+        <v>424.83870967741933</v>
+      </c>
+      <c r="V40">
+        <f t="shared" ref="V40:V50" si="15">D40/M40</f>
+        <v>432.10714285714278</v>
+      </c>
+      <c r="W40">
+        <f t="shared" ref="W40:W50" si="16">E40/N40</f>
+        <v>181.93103448275863</v>
+      </c>
+      <c r="X40">
+        <f t="shared" ref="X40:X50" si="17">F40/O40</f>
+        <v>478.56249999999994</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" ref="Y40:Y50" si="18">G40/P40</f>
+        <v>374.6</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" ref="Z40:Z50" si="19">H40/Q40</f>
+        <v>492.00000000000006</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" ref="AA40:AA50" si="20">I40/R40</f>
+        <v>314.9677419354839</v>
+      </c>
+      <c r="AC40">
+        <f>AVERAGE(U40:AA50)</f>
+        <v>482.0426978724833</v>
+      </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>20</v>
       </c>
@@ -3992,8 +4957,39 @@
       <c r="R41">
         <v>0.28999999999999998</v>
       </c>
+      <c r="T41" t="s">
+        <v>20</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="14"/>
+        <v>430.35483870967744</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="15"/>
+        <v>415.60714285714283</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="16"/>
+        <v>197.40740740740739</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="17"/>
+        <v>532.24137931034488</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="18"/>
+        <v>383.24137931034488</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="19"/>
+        <v>459.31034482758622</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="20"/>
+        <v>304.9655172413793</v>
+      </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>21</v>
       </c>
@@ -4042,8 +5038,39 @@
       <c r="R42">
         <v>0.3</v>
       </c>
+      <c r="T42" t="s">
+        <v>21</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="14"/>
+        <v>349.36842105263156</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="15"/>
+        <v>426.71428571428567</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="16"/>
+        <v>175.6875</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="17"/>
+        <v>385.3</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="18"/>
+        <v>291.18421052631578</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="19"/>
+        <v>470.00000000000006</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="20"/>
+        <v>303.56666666666666</v>
+      </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>22</v>
       </c>
@@ -4092,8 +5119,39 @@
       <c r="R43">
         <v>0.28999999999999998</v>
       </c>
+      <c r="T43" t="s">
+        <v>22</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="14"/>
+        <v>310.12765957446811</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="15"/>
+        <v>439.75862068965523</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="16"/>
+        <v>206.21428571428569</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="17"/>
+        <v>305.36</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="18"/>
+        <v>230.6</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" si="19"/>
+        <v>463.33333333333337</v>
+      </c>
+      <c r="AA43">
+        <f t="shared" si="20"/>
+        <v>329.58620689655174</v>
+      </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>23</v>
       </c>
@@ -4142,8 +5200,39 @@
       <c r="R44">
         <v>0.28000000000000003</v>
       </c>
+      <c r="T44" t="s">
+        <v>23</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="14"/>
+        <v>258.07547169811318</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="15"/>
+        <v>407.96774193548384</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="16"/>
+        <v>207.75</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="17"/>
+        <v>269.69090909090909</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="18"/>
+        <v>202.66666666666666</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="19"/>
+        <v>493.48275862068971</v>
+      </c>
+      <c r="AA44">
+        <f t="shared" si="20"/>
+        <v>349.28571428571422</v>
+      </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>24</v>
       </c>
@@ -4192,8 +5281,39 @@
       <c r="R45">
         <v>0.28999999999999998</v>
       </c>
+      <c r="T45" t="s">
+        <v>24</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="14"/>
+        <v>273.56363636363636</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="15"/>
+        <v>460.53571428571422</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="16"/>
+        <v>211.17857142857142</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="17"/>
+        <v>293.46031746031747</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" si="18"/>
+        <v>223.4</v>
+      </c>
+      <c r="Z45">
+        <f t="shared" si="19"/>
+        <v>532.75862068965523</v>
+      </c>
+      <c r="AA45">
+        <f t="shared" si="20"/>
+        <v>353.72413793103448</v>
+      </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>25</v>
       </c>
@@ -4242,8 +5362,39 @@
       <c r="R46">
         <v>0.31</v>
       </c>
+      <c r="T46" t="s">
+        <v>25</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="14"/>
+        <v>322.13333333333333</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="15"/>
+        <v>529.03571428571422</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="16"/>
+        <v>224.06896551724139</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="17"/>
+        <v>421.82089552238801</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="18"/>
+        <v>395.75384615384615</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="19"/>
+        <v>771.12903225806451</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="20"/>
+        <v>489.48387096774195</v>
+      </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>26</v>
       </c>
@@ -4292,8 +5443,39 @@
       <c r="R47">
         <v>0.3</v>
       </c>
+      <c r="T47" t="s">
+        <v>26</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="14"/>
+        <v>310.53968253968253</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="15"/>
+        <v>859.27586206896558</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="16"/>
+        <v>279.24137931034488</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="17"/>
+        <v>576.53846153846155</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="18"/>
+        <v>452.328125</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="19"/>
+        <v>966.54545454545439</v>
+      </c>
+      <c r="AA47">
+        <f t="shared" si="20"/>
+        <v>692.13333333333333</v>
+      </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>27</v>
       </c>
@@ -4342,8 +5524,39 @@
       <c r="R48">
         <v>0.35</v>
       </c>
+      <c r="T48" t="s">
+        <v>27</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="14"/>
+        <v>322.72499999999997</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="15"/>
+        <v>895.58064516129036</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="16"/>
+        <v>378.75757575757575</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="17"/>
+        <v>534.67532467532465</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="18"/>
+        <v>540.55384615384617</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="19"/>
+        <v>1422.5675675675677</v>
+      </c>
+      <c r="AA48">
+        <f t="shared" si="20"/>
+        <v>833.97142857142853</v>
+      </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>28</v>
       </c>
@@ -4392,8 +5605,39 @@
       <c r="R49">
         <v>0.4</v>
       </c>
+      <c r="T49" t="s">
+        <v>28</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="14"/>
+        <v>340.62886597938149</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="15"/>
+        <v>1053.8947368421052</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="16"/>
+        <v>342.18421052631578</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="17"/>
+        <v>457.18279569892474</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="18"/>
+        <v>458.57499999999999</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="19"/>
+        <v>1436.8999999999999</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="20"/>
+        <v>999.95</v>
+      </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>29</v>
       </c>
@@ -4442,13 +5686,44 @@
       <c r="R50">
         <v>0.4</v>
       </c>
+      <c r="T50" t="s">
+        <v>29</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="14"/>
+        <v>352.28571428571428</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="15"/>
+        <v>1188.8974358974358</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="16"/>
+        <v>389.75675675675677</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="17"/>
+        <v>497.77319587628864</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" si="18"/>
+        <v>487.42352941176472</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" si="19"/>
+        <v>1122.8245614035088</v>
+      </c>
+      <c r="AA50">
+        <f>I50/R50</f>
+        <v>1123.675</v>
+      </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>13</v>
       </c>
@@ -4492,7 +5767,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>17</v>
       </c>
@@ -4536,7 +5811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>18</v>
       </c>
@@ -4556,7 +5831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -4606,7 +5881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>19</v>
       </c>
@@ -4656,7 +5931,7 @@
         <v>10.88</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>20</v>
       </c>
@@ -4706,7 +5981,7 @@
         <v>15.04</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>21</v>
       </c>
@@ -4756,7 +6031,7 @@
         <v>33.369999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>22</v>
       </c>
@@ -4806,7 +6081,7 @@
         <v>46.51</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>23</v>
       </c>
@@ -4856,7 +6131,7 @@
         <v>44.59</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>24</v>
       </c>
@@ -4906,7 +6181,7 @@
         <v>45.1</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>25</v>
       </c>
@@ -5166,7 +6441,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:I16 L6:R16">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5178,7 +6453,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:I33 L23:R33">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5190,6 +6465,54 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:I50 L40:R50">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L58:R68 C58:I68">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U6:AA16 AC6">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U40:AA49 U23:AA33 U50:AA50">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -5201,7 +6524,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L58:R68 C58:I68">
+  <conditionalFormatting sqref="AC23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5213,7 +6536,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
+  <conditionalFormatting sqref="AC40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -16203,7 +17526,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:AJ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>

</xml_diff>